<commit_message>
need to make variables for density slices
</commit_message>
<xml_diff>
--- a/data/ctd-cnv/KM1919/P2_2019/primary_chl/Station20_integrated_PCM.xlsx
+++ b/data/ctd-cnv/KM1919/P2_2019/primary_chl/Station20_integrated_PCM.xlsx
@@ -9,6 +9,7 @@
   </bookViews>
   <sheets>
     <sheet name="Station20_integrated_PCM" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="matlab input" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -248,9 +249,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
+    <numFmt numFmtId="166" formatCode="0.00"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -316,12 +318,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -342,10 +348,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G36"/>
+  <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="J32" activeCellId="0" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -424,6 +430,14 @@
       <c r="G3" s="0" t="n">
         <v>3690.297</v>
       </c>
+      <c r="H3" s="2" t="n">
+        <f aca="false">D3-$D$2</f>
+        <v>0</v>
+      </c>
+      <c r="I3" s="2" t="n">
+        <f aca="false">G4-$G$3</f>
+        <v>1996.185</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
@@ -439,13 +453,21 @@
         <v>744918.459479167</v>
       </c>
       <c r="E4" s="0" t="n">
-        <v>57.7095</v>
+        <v>35.3422</v>
       </c>
       <c r="F4" s="0" t="n">
-        <v>26594.2224</v>
+        <v>5529.8537</v>
       </c>
       <c r="G4" s="0" t="n">
-        <v>5969.36</v>
+        <v>5686.482</v>
+      </c>
+      <c r="H4" s="2" t="n">
+        <f aca="false">D4-$D$2</f>
+        <v>1.89587962965015</v>
+      </c>
+      <c r="I4" s="2" t="n">
+        <f aca="false">G5-$G$3</f>
+        <v>1200.765</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -462,13 +484,21 @@
         <v>744918.993101852</v>
       </c>
       <c r="E5" s="0" t="n">
-        <v>66.5312</v>
+        <v>39.1988</v>
       </c>
       <c r="F5" s="0" t="n">
-        <v>26773.4716</v>
+        <v>5221.2258</v>
       </c>
       <c r="G5" s="0" t="n">
-        <v>5158.425</v>
+        <v>4891.062</v>
+      </c>
+      <c r="H5" s="2" t="n">
+        <f aca="false">D5-$D$2</f>
+        <v>2.42950231488794</v>
+      </c>
+      <c r="I5" s="2" t="n">
+        <f aca="false">G6-$G$3</f>
+        <v>1315.778</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -485,13 +515,21 @@
         <v>744920.360914352</v>
       </c>
       <c r="E6" s="0" t="n">
-        <v>107.7809</v>
+        <v>35.2071</v>
       </c>
       <c r="F6" s="0" t="n">
-        <v>96023.5814</v>
+        <v>5533.8321</v>
       </c>
       <c r="G6" s="0" t="n">
-        <v>7054.908</v>
+        <v>5006.075</v>
+      </c>
+      <c r="H6" s="2" t="n">
+        <f aca="false">D6-$D$2</f>
+        <v>3.79731481487397</v>
+      </c>
+      <c r="I6" s="2" t="n">
+        <f aca="false">G7-$G$3</f>
+        <v>639.429</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -508,13 +546,21 @@
         <v>744920.585439815</v>
       </c>
       <c r="E7" s="0" t="n">
-        <v>100.4304</v>
+        <v>32.8385</v>
       </c>
       <c r="F7" s="0" t="n">
-        <v>94117.0924</v>
+        <v>5438.7797</v>
       </c>
       <c r="G7" s="0" t="n">
-        <v>6224.446</v>
+        <v>4329.726</v>
+      </c>
+      <c r="H7" s="2" t="n">
+        <f aca="false">D7-$D$2</f>
+        <v>4.02184027782641</v>
+      </c>
+      <c r="I7" s="2" t="n">
+        <f aca="false">G8-$G$3</f>
+        <v>2204.21</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -531,13 +577,21 @@
         <v>744920.901643518</v>
       </c>
       <c r="E8" s="0" t="n">
-        <v>83.6852</v>
+        <v>49.7302</v>
       </c>
       <c r="F8" s="0" t="n">
-        <v>44836.603</v>
+        <v>5811.2156</v>
       </c>
       <c r="G8" s="0" t="n">
-        <v>6322.003</v>
+        <v>5894.507</v>
+      </c>
+      <c r="H8" s="2" t="n">
+        <f aca="false">D8-$D$2</f>
+        <v>4.33804398146458</v>
+      </c>
+      <c r="I8" s="2" t="n">
+        <f aca="false">G9-$G$3</f>
+        <v>3643.257</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -554,13 +608,21 @@
         <v>744922.593356482</v>
       </c>
       <c r="E9" s="0" t="n">
-        <v>61.2967</v>
+        <v>44.3451</v>
       </c>
       <c r="F9" s="0" t="n">
-        <v>15347.4816</v>
+        <v>6213.1971</v>
       </c>
       <c r="G9" s="0" t="n">
-        <v>7461.636</v>
+        <v>7333.554</v>
+      </c>
+      <c r="H9" s="2" t="n">
+        <f aca="false">D9-$D$2</f>
+        <v>6.02975694451015</v>
+      </c>
+      <c r="I9" s="2" t="n">
+        <f aca="false">G10-$G$3</f>
+        <v>3587.006</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -577,13 +639,21 @@
         <v>744922.818298611</v>
       </c>
       <c r="E10" s="0" t="n">
-        <v>89.3837</v>
+        <v>43.5503</v>
       </c>
       <c r="F10" s="0" t="n">
-        <v>65347.5107</v>
+        <v>6194.5132</v>
       </c>
       <c r="G10" s="0" t="n">
-        <v>7943.816</v>
+        <v>7277.303</v>
+      </c>
+      <c r="H10" s="2" t="n">
+        <f aca="false">D10-$D$2</f>
+        <v>6.25469907408115</v>
+      </c>
+      <c r="I10" s="2" t="n">
+        <f aca="false">G11-$G$3</f>
+        <v>2878.524</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -600,13 +670,21 @@
         <v>744922.950659722</v>
       </c>
       <c r="E11" s="0" t="n">
-        <v>118.5174</v>
+        <v>38.3841</v>
       </c>
       <c r="F11" s="0" t="n">
-        <v>114689.1344</v>
+        <v>5805.3173</v>
       </c>
       <c r="G11" s="0" t="n">
-        <v>11533.641</v>
+        <v>6568.821</v>
+      </c>
+      <c r="H11" s="2" t="n">
+        <f aca="false">D11-$D$2</f>
+        <v>6.38706018519588</v>
+      </c>
+      <c r="I11" s="2" t="n">
+        <f aca="false">G12-$G$3</f>
+        <v>2926.201</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -623,13 +701,21 @@
         <v>744924.074328704</v>
       </c>
       <c r="E12" s="0" t="n">
-        <v>125.3863</v>
+        <v>41.3419</v>
       </c>
       <c r="F12" s="0" t="n">
-        <v>119485.4325</v>
+        <v>6004.2921</v>
       </c>
       <c r="G12" s="0" t="n">
-        <v>12619.73</v>
+        <v>6616.498</v>
+      </c>
+      <c r="H12" s="2" t="n">
+        <f aca="false">D12-$D$2</f>
+        <v>7.51072916667908</v>
+      </c>
+      <c r="I12" s="2" t="n">
+        <f aca="false">G13-$G$3</f>
+        <v>3850.974</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -646,13 +732,21 @@
         <v>744924.319479167</v>
       </c>
       <c r="E13" s="0" t="n">
-        <v>75.1198</v>
+        <v>39.9904</v>
       </c>
       <c r="F13" s="0" t="n">
-        <v>45506.2539</v>
+        <v>6805.9705</v>
       </c>
       <c r="G13" s="0" t="n">
-        <v>8046.352</v>
+        <v>7541.271</v>
+      </c>
+      <c r="H13" s="2" t="n">
+        <f aca="false">D13-$D$2</f>
+        <v>7.75587962963618</v>
+      </c>
+      <c r="I13" s="2" t="n">
+        <f aca="false">G14-$G$3</f>
+        <v>4872.611</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -669,13 +763,21 @@
         <v>744924.701481481</v>
       </c>
       <c r="E14" s="0" t="n">
-        <v>61.9578</v>
+        <v>42.9352</v>
       </c>
       <c r="F14" s="0" t="n">
-        <v>20280.4516</v>
+        <v>6197.2893</v>
       </c>
       <c r="G14" s="0" t="n">
-        <v>8802.399</v>
+        <v>8562.908</v>
+      </c>
+      <c r="H14" s="2" t="n">
+        <f aca="false">D14-$D$2</f>
+        <v>8.13788194442168</v>
+      </c>
+      <c r="I14" s="2" t="n">
+        <f aca="false">G15-$G$3</f>
+        <v>4096.446</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -692,13 +794,21 @@
         <v>744924.864918981</v>
       </c>
       <c r="E15" s="0" t="n">
-        <v>78.9871</v>
+        <v>45.5347</v>
       </c>
       <c r="F15" s="0" t="n">
-        <v>44872.2796</v>
+        <v>5784.1948</v>
       </c>
       <c r="G15" s="0" t="n">
-        <v>8238.555</v>
+        <v>7786.743</v>
+      </c>
+      <c r="H15" s="2" t="n">
+        <f aca="false">D15-$D$2</f>
+        <v>8.30131944443565</v>
+      </c>
+      <c r="I15" s="2" t="n">
+        <f aca="false">G16-$G$3</f>
+        <v>5091.097</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -715,13 +825,21 @@
         <v>744926.044490741</v>
       </c>
       <c r="E16" s="0" t="n">
-        <v>57.4993</v>
+        <v>43.3187</v>
       </c>
       <c r="F16" s="0" t="n">
-        <v>15260.54</v>
+        <v>6664.5777</v>
       </c>
       <c r="G16" s="0" t="n">
-        <v>8909.025</v>
+        <v>8781.394</v>
+      </c>
+      <c r="H16" s="2" t="n">
+        <f aca="false">D16-$D$2</f>
+        <v>9.48089120374061</v>
+      </c>
+      <c r="I16" s="2" t="n">
+        <f aca="false">G17-$G$3</f>
+        <v>3878.077</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -738,13 +856,21 @@
         <v>744926.294965278</v>
       </c>
       <c r="E17" s="0" t="n">
-        <v>56.2056</v>
+        <v>38.3542</v>
       </c>
       <c r="F17" s="0" t="n">
-        <v>15602.5467</v>
+        <v>6692.7836</v>
       </c>
       <c r="G17" s="0" t="n">
-        <v>7708.544</v>
+        <v>7568.374</v>
+      </c>
+      <c r="H17" s="2" t="n">
+        <f aca="false">D17-$D$2</f>
+        <v>9.73136574076489</v>
+      </c>
+      <c r="I17" s="2" t="n">
+        <f aca="false">G18-$G$3</f>
+        <v>4022.534</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -761,13 +887,21 @@
         <v>744926.555891204</v>
       </c>
       <c r="E18" s="0" t="n">
-        <v>57.0012</v>
+        <v>42.7906</v>
       </c>
       <c r="F18" s="0" t="n">
-        <v>15208.3099</v>
+        <v>6097.5067</v>
       </c>
       <c r="G18" s="0" t="n">
-        <v>7847.324</v>
+        <v>7712.831</v>
+      </c>
+      <c r="H18" s="2" t="n">
+        <f aca="false">D18-$D$2</f>
+        <v>9.99229166668374</v>
+      </c>
+      <c r="I18" s="2" t="n">
+        <f aca="false">G19-$G$3</f>
+        <v>3406.888</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -784,13 +918,21 @@
         <v>744926.666469907</v>
       </c>
       <c r="E19" s="0" t="n">
-        <v>50.1083</v>
+        <v>36.3536</v>
       </c>
       <c r="F19" s="0" t="n">
-        <v>14615.4372</v>
+        <v>6300.9881</v>
       </c>
       <c r="G19" s="0" t="n">
-        <v>7220.336</v>
+        <v>7097.185</v>
+      </c>
+      <c r="H19" s="2" t="n">
+        <f aca="false">D19-$D$2</f>
+        <v>10.1028703703778</v>
+      </c>
+      <c r="I19" s="2" t="n">
+        <f aca="false">G20-$G$3</f>
+        <v>5229.415</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -807,13 +949,21 @@
         <v>744926.788784722</v>
       </c>
       <c r="E20" s="0" t="n">
-        <v>60.6235</v>
+        <v>48.1295</v>
       </c>
       <c r="F20" s="0" t="n">
-        <v>15791.9289</v>
+        <v>6681.1926</v>
       </c>
       <c r="G20" s="0" t="n">
-        <v>9070.543</v>
+        <v>8919.712</v>
+      </c>
+      <c r="H20" s="2" t="n">
+        <f aca="false">D20-$D$2</f>
+        <v>10.2251851852052</v>
+      </c>
+      <c r="I20" s="2" t="n">
+        <f aca="false">G21-$G$3</f>
+        <v>3938.08</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -830,13 +980,21 @@
         <v>744926.924050926</v>
       </c>
       <c r="E21" s="0" t="n">
-        <v>70.058</v>
+        <v>42.9438</v>
       </c>
       <c r="F21" s="0" t="n">
-        <v>35495.5205</v>
+        <v>5898.7326</v>
       </c>
       <c r="G21" s="0" t="n">
-        <v>7997.861</v>
+        <v>7628.377</v>
+      </c>
+      <c r="H21" s="2" t="n">
+        <f aca="false">D21-$D$2</f>
+        <v>10.3604513888713</v>
+      </c>
+      <c r="I21" s="2" t="n">
+        <f aca="false">G22-$G$3</f>
+        <v>4134.622</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -853,13 +1011,21 @@
         <v>744928.049027778</v>
       </c>
       <c r="E22" s="0" t="n">
-        <v>57.2566</v>
+        <v>43.3484</v>
       </c>
       <c r="F22" s="0" t="n">
-        <v>14923.9835</v>
+        <v>6295.9843</v>
       </c>
       <c r="G22" s="0" t="n">
-        <v>7953.786</v>
+        <v>7824.919</v>
+      </c>
+      <c r="H22" s="2" t="n">
+        <f aca="false">D22-$D$2</f>
+        <v>11.4854282407323</v>
+      </c>
+      <c r="I22" s="2" t="n">
+        <f aca="false">G23-$G$3</f>
+        <v>3618.777</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -876,13 +1042,21 @@
         <v>744928.324884259</v>
       </c>
       <c r="E23" s="0" t="n">
-        <v>67.934</v>
+        <v>40.2526</v>
       </c>
       <c r="F23" s="0" t="n">
-        <v>30441.8505</v>
+        <v>5908.3751</v>
       </c>
       <c r="G23" s="0" t="n">
-        <v>7641.13</v>
+        <v>7309.074</v>
+      </c>
+      <c r="H23" s="2" t="n">
+        <f aca="false">D23-$D$2</f>
+        <v>11.7612847222481</v>
+      </c>
+      <c r="I23" s="2" t="n">
+        <f aca="false">G24-$G$3</f>
+        <v>2502.225</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -899,13 +1073,21 @@
         <v>744928.480868056</v>
       </c>
       <c r="E24" s="0" t="n">
-        <v>67.652</v>
+        <v>33.9291</v>
       </c>
       <c r="F24" s="0" t="n">
-        <v>34926.5232</v>
+        <v>5619.4021</v>
       </c>
       <c r="G24" s="0" t="n">
-        <v>6535.573</v>
+        <v>6192.522</v>
+      </c>
+      <c r="H24" s="2" t="n">
+        <f aca="false">D24-$D$2</f>
+        <v>11.9172685185913</v>
+      </c>
+      <c r="I24" s="2" t="n">
+        <f aca="false">G25-$G$3</f>
+        <v>4304.368</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -922,13 +1104,21 @@
         <v>744928.594236111</v>
       </c>
       <c r="E25" s="0" t="n">
-        <v>59.5096</v>
+        <v>39.7258</v>
       </c>
       <c r="F25" s="0" t="n">
-        <v>14929.3932</v>
+        <v>6504.3323</v>
       </c>
       <c r="G25" s="0" t="n">
-        <v>8103.999</v>
+        <v>7994.665</v>
+      </c>
+      <c r="H25" s="2" t="n">
+        <f aca="false">D25-$D$2</f>
+        <v>12.0306365741417</v>
+      </c>
+      <c r="I25" s="2" t="n">
+        <f aca="false">G26-$G$3</f>
+        <v>4550.913</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -945,13 +1135,21 @@
         <v>744928.800706018</v>
       </c>
       <c r="E26" s="0" t="n">
-        <v>60.5628</v>
+        <v>46.5652</v>
       </c>
       <c r="F26" s="0" t="n">
-        <v>15700.1971</v>
+        <v>7085.6091</v>
       </c>
       <c r="G26" s="0" t="n">
-        <v>8376.274</v>
+        <v>8241.21</v>
+      </c>
+      <c r="H26" s="2" t="n">
+        <f aca="false">D26-$D$2</f>
+        <v>12.2371064814506</v>
+      </c>
+      <c r="I26" s="2" t="n">
+        <f aca="false">G27-$G$3</f>
+        <v>5004.102</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -968,13 +1166,21 @@
         <v>744932.006921296</v>
       </c>
       <c r="E27" s="0" t="n">
-        <v>58.2807</v>
+        <v>43.3622</v>
       </c>
       <c r="F27" s="0" t="n">
-        <v>15490.6096</v>
+        <v>6684.064</v>
       </c>
       <c r="G27" s="0" t="n">
-        <v>8823.714</v>
+        <v>8694.399</v>
+      </c>
+      <c r="H27" s="2" t="n">
+        <f aca="false">D27-$D$2</f>
+        <v>15.4433217592305</v>
+      </c>
+      <c r="I27" s="2" t="n">
+        <f aca="false">G28-$G$3</f>
+        <v>4299.489</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -991,13 +1197,21 @@
         <v>744932.201319444</v>
       </c>
       <c r="E28" s="0" t="n">
-        <v>55.1446</v>
+        <v>36.4633</v>
       </c>
       <c r="F28" s="0" t="n">
-        <v>15665.562</v>
+        <v>5986.7851</v>
       </c>
       <c r="G28" s="0" t="n">
-        <v>8159.375</v>
+        <v>7989.786</v>
+      </c>
+      <c r="H28" s="2" t="n">
+        <f aca="false">D28-$D$2</f>
+        <v>15.6377199074486</v>
+      </c>
+      <c r="I28" s="2" t="n">
+        <f aca="false">G29-$G$3</f>
+        <v>5249.313</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1014,13 +1228,21 @@
         <v>744932.516863426</v>
       </c>
       <c r="E29" s="0" t="n">
-        <v>63.2927</v>
+        <v>42.1993</v>
       </c>
       <c r="F29" s="0" t="n">
-        <v>27045.7317</v>
+        <v>6972.95</v>
       </c>
       <c r="G29" s="0" t="n">
-        <v>9176.788</v>
+        <v>8939.61</v>
+      </c>
+      <c r="H29" s="2" t="n">
+        <f aca="false">D29-$D$2</f>
+        <v>15.9532638889505</v>
+      </c>
+      <c r="I29" s="2" t="n">
+        <f aca="false">G30-$G$3</f>
+        <v>5528.566</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1037,13 +1259,21 @@
         <v>744932.797453704</v>
       </c>
       <c r="E30" s="0" t="n">
-        <v>80.7831</v>
+        <v>45.7997</v>
       </c>
       <c r="F30" s="0" t="n">
-        <v>46189.4977</v>
+        <v>7053.2492</v>
       </c>
       <c r="G30" s="0" t="n">
-        <v>9692.837</v>
+        <v>9218.863</v>
+      </c>
+      <c r="H30" s="2" t="n">
+        <f aca="false">D30-$D$2</f>
+        <v>16.2338541666977</v>
+      </c>
+      <c r="I30" s="2" t="n">
+        <f aca="false">G31-$G$3</f>
+        <v>5592.579</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1060,13 +1290,21 @@
         <v>744932.962118056</v>
       </c>
       <c r="E31" s="0" t="n">
-        <v>67.0015</v>
+        <v>47.8637</v>
       </c>
       <c r="F31" s="0" t="n">
-        <v>26992.7838</v>
+        <v>7048.8991</v>
       </c>
       <c r="G31" s="0" t="n">
-        <v>9517.682</v>
+        <v>9282.876</v>
+      </c>
+      <c r="H31" s="2" t="n">
+        <f aca="false">D31-$D$2</f>
+        <v>16.3985185185447</v>
+      </c>
+      <c r="I31" s="2" t="n">
+        <f aca="false">G32-$G$3</f>
+        <v>6711.685</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1083,13 +1321,21 @@
         <v>744934.104594907</v>
       </c>
       <c r="E32" s="0" t="n">
-        <v>76.7948</v>
+        <v>55.1072</v>
       </c>
       <c r="F32" s="0" t="n">
-        <v>30844.2801</v>
+        <v>7335.7076</v>
       </c>
       <c r="G32" s="0" t="n">
-        <v>10730.192</v>
+        <v>10401.982</v>
+      </c>
+      <c r="H32" s="2" t="n">
+        <f aca="false">D32-$D$2</f>
+        <v>17.5409953703638</v>
+      </c>
+      <c r="I32" s="2" t="n">
+        <f aca="false">G33-$G$3</f>
+        <v>5227.136</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1106,13 +1352,21 @@
         <v>744934.438530093</v>
       </c>
       <c r="E33" s="0" t="n">
-        <v>56.1697</v>
+        <v>36.9545</v>
       </c>
       <c r="F33" s="0" t="n">
-        <v>15427.6164</v>
+        <v>5671.9952</v>
       </c>
       <c r="G33" s="0" t="n">
-        <v>9085.055</v>
+        <v>8917.433</v>
+      </c>
+      <c r="H33" s="2" t="n">
+        <f aca="false">D33-$D$2</f>
+        <v>17.874930555583</v>
+      </c>
+      <c r="I33" s="2" t="n">
+        <f aca="false">G34-$G$3</f>
+        <v>6946.462</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1129,13 +1383,21 @@
         <v>744934.551064815</v>
       </c>
       <c r="E34" s="0" t="n">
-        <v>73.7703</v>
+        <v>41.5817</v>
       </c>
       <c r="F34" s="0" t="n">
-        <v>34621.3019</v>
+        <v>7252.8361</v>
       </c>
       <c r="G34" s="0" t="n">
-        <v>11008.696</v>
+        <v>10636.759</v>
+      </c>
+      <c r="H34" s="2" t="n">
+        <f aca="false">D34-$D$2</f>
+        <v>17.9874652777798</v>
+      </c>
+      <c r="I34" s="2" t="n">
+        <f aca="false">G35-$G$3</f>
+        <v>5605.123</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1152,13 +1414,21 @@
         <v>744934.826145833</v>
       </c>
       <c r="E35" s="0" t="n">
-        <v>156.4772</v>
+        <v>43.3686</v>
       </c>
       <c r="F35" s="0" t="n">
-        <v>169551.0435</v>
+        <v>6260.4922</v>
       </c>
       <c r="G35" s="0" t="n">
-        <v>38274.883</v>
+        <v>9295.42</v>
+      </c>
+      <c r="H35" s="2" t="n">
+        <f aca="false">D35-$D$2</f>
+        <v>18.2625462963479</v>
+      </c>
+      <c r="I35" s="2" t="n">
+        <f aca="false">G36-$G$3</f>
+        <v>6445.479</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1175,13 +1445,21 @@
         <v>744936.21443287</v>
       </c>
       <c r="E36" s="0" t="n">
-        <v>89.993</v>
+        <v>45.1225</v>
       </c>
       <c r="F36" s="0" t="n">
-        <v>65665.2249</v>
+        <v>7536.8948</v>
       </c>
       <c r="G36" s="0" t="n">
-        <v>10783.864</v>
+        <v>10135.776</v>
+      </c>
+      <c r="H36" s="2" t="n">
+        <f aca="false">D36-$D$2</f>
+        <v>19.6508333333768</v>
+      </c>
+      <c r="I36" s="2" t="n">
+        <f aca="false">G37-$G$3</f>
+        <v>-3690.297</v>
       </c>
     </row>
   </sheetData>
@@ -1193,4 +1471,27 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>